<commit_message>
we just use actual bools
</commit_message>
<xml_diff>
--- a/examples/data.xlsx
+++ b/examples/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/code/projects/nvmbuilder/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/code/projects/mint/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259C8242-0CD5-C148-8C6D-EEF28A851E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88ED2DCA-4DF6-F84A-B747-427CA78F15CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>#DebugCoefficients</t>
+  </si>
+  <si>
+    <t>boolean</t>
   </si>
 </sst>
 </file>
@@ -553,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81175D9F-030E-4648-B932-899D2D945A10}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,6 +750,20 @@
       </c>
       <c r="B27" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add boolean handling in preparation for bitmaps (#16)
* feat: Implement bitmap leaf entries for bit packing

Co-authored-by: t <t@tomrford.com>

* Refactor: Implement bitmap leaf type support

Co-authored-by: t <t@tomrford.com>

* Refactor: Improve bitmap leaf implementation and validation

Co-authored-by: t <t@tomrford.com>

* feat: Add boolean support to DataValue and conversions

This change introduces boolean support to DataValue, allowing for true/false values. It also enhances conversions to handle boolean types, enabling their use in various contexts like configuration files and data streams.

Co-authored-by: t <t@tomrford.com>

* improving agents.md

* we just use actual bools

* bools are feature complete

* removing the docs for first merge

---------

Co-authored-by: Cursor Agent <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/examples/data.xlsx
+++ b/examples/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/code/projects/nvmbuilder/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/code/projects/mint/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259C8242-0CD5-C148-8C6D-EEF28A851E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88ED2DCA-4DF6-F84A-B747-427CA78F15CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>#DebugCoefficients</t>
+  </si>
+  <si>
+    <t>boolean</t>
   </si>
 </sst>
 </file>
@@ -553,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81175D9F-030E-4648-B932-899D2D945A10}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,6 +750,20 @@
       </c>
       <c r="B27" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding bitmap support (#17)
* readding docs as context

* adding structures needed for bitmaps

* working bitfields

* some comment cleanup
</commit_message>
<xml_diff>
--- a/examples/data.xlsx
+++ b/examples/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/code/projects/mint/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88ED2DCA-4DF6-F84A-B747-427CA78F15CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DB604C-3C3B-B04A-92A5-199F7166C2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -177,6 +177,33 @@
   </si>
   <si>
     <t>boolean</t>
+  </si>
+  <si>
+    <t>BitmapTestCount</t>
+  </si>
+  <si>
+    <t>AllowDebug</t>
+  </si>
+  <si>
+    <t>ModeSelect</t>
+  </si>
+  <si>
+    <t>RegionCode</t>
+  </si>
+  <si>
+    <t>PowerGood</t>
+  </si>
+  <si>
+    <t>FanRunning</t>
+  </si>
+  <si>
+    <t>ErrorCode</t>
+  </si>
+  <si>
+    <t>HwRevision</t>
+  </si>
+  <si>
+    <t>BitmapCheckVal</t>
   </si>
 </sst>
 </file>
@@ -219,9 +246,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81175D9F-030E-4648-B932-899D2D945A10}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,6 +792,78 @@
       </c>
       <c r="D29" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="2">
+        <v>305419896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>